<commit_message>
GA FOREVAAA AND EVAAA
</commit_message>
<xml_diff>
--- a/Zeus/data/TSP/Results/Comparison.xlsx
+++ b/Zeus/data/TSP/Results/Comparison.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="132">
   <si>
     <t>FileName</t>
   </si>
@@ -406,6 +406,15 @@
   </si>
   <si>
     <t>1.279s</t>
+  </si>
+  <si>
+    <t>6.764s</t>
+  </si>
+  <si>
+    <t>29.889s</t>
+  </si>
+  <si>
+    <t>0.37s</t>
   </si>
 </sst>
 </file>
@@ -839,19 +848,19 @@
         <v>3320.119873046875</v>
       </c>
       <c r="D2" t="n">
-        <v>2895.980224609375</v>
+        <v>2871.75244140625</v>
       </c>
       <c r="E2" t="n">
-        <v>12.77482936326233</v>
+        <v>13.504555521640194</v>
       </c>
       <c r="F2" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="G2" t="n">
         <v>30.0</v>
       </c>
       <c r="H2" t="n">
-        <v>250.0</v>
+        <v>300.0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -865,19 +874,19 @@
         <v>2529.9921875</v>
       </c>
       <c r="D3" t="n">
-        <v>2128.58447265625</v>
+        <v>2162.1923828125</v>
       </c>
       <c r="E3" t="n">
-        <v>15.865966575983748</v>
+        <v>14.53758657851587</v>
       </c>
       <c r="F3" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="G3" t="n">
         <v>30.0</v>
       </c>
       <c r="H3" t="n">
-        <v>250.0</v>
+        <v>300.0</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -891,19 +900,19 @@
         <v>39306.31640625</v>
       </c>
       <c r="D4" t="n">
-        <v>32358.716796875</v>
+        <v>32272.44921875</v>
       </c>
       <c r="E4" t="n">
-        <v>17.675529646604783</v>
+        <v>17.895004748859044</v>
       </c>
       <c r="F4" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="G4" t="n">
         <v>30.0</v>
       </c>
       <c r="H4" t="n">
-        <v>250.0</v>
+        <v>300.0</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>